<commit_message>
Logbook : Reflectieverslag Lukasz
</commit_message>
<xml_diff>
--- a/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_lukasz.xlsx
+++ b/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_lukasz.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7680" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="8136" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lukasz" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,9 +102,6 @@
     <t>Donderdag:</t>
   </si>
   <si>
-    <t>Vrijdag:</t>
-  </si>
-  <si>
     <t>Zaterdag:</t>
   </si>
   <si>
@@ -292,12 +289,15 @@
   </si>
   <si>
     <t>Donderdag: Presetatie voorberijding</t>
+  </si>
+  <si>
+    <t>Vrijdag: Reflectieverslag en logbook bijgewerkt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -797,32 +797,71 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -830,65 +869,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1174,11 +1174,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,11 +1187,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="3" spans="1:17" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
@@ -1236,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="7">
         <v>3</v>
@@ -1245,16 +1245,16 @@
         <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="7">
         <v>2</v>
       </c>
-      <c r="O5" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="38"/>
+      <c r="O5" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="39"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
@@ -1267,26 +1267,26 @@
         <v>3</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="O6" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="47"/>
+      <c r="O6" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="50"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
@@ -1299,7 +1299,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="7">
         <v>3</v>
@@ -1308,16 +1308,16 @@
         <v>3</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="O7" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="41"/>
+        <v>39</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="42"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
@@ -1330,7 +1330,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="7">
         <v>3</v>
@@ -1339,16 +1339,16 @@
         <v>3</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="O8" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="41"/>
+        <v>39</v>
+      </c>
+      <c r="O8" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="42"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
@@ -1376,11 +1376,11 @@
         <v>6</v>
       </c>
       <c r="K9" s="8"/>
-      <c r="O9" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="41"/>
+      <c r="O9" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
@@ -1403,11 +1403,11 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="O10" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="44"/>
+      <c r="O10" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="47"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C11" s="9" t="s">
@@ -1436,11 +1436,19 @@
       <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>3</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
@@ -1495,13 +1503,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="12">
         <f>SUM((D5,D6,D7,D8,D9,D10,D11,D12,E5,E6,E7,E8,E9,E10,E11,E12,F5,F6,F7,F8,F9,F10,F11,F12,G5,G6,G7,G8,G9,G10,G11,G12,H5,H6,H7,H8,H9,H10,H11,H12,I5,I6,I7,I8,I9,I10,I11,I12,J5,J6,J7,J8,J9,J10,J11,J12,D13,D14,E13,E14,F13,F14,G13,G14,H13,H14,I13,I14,J13,J14))</f>
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1551,22 +1559,22 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="29"/>
+      <c r="C20" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="21" t="s">
-        <v>42</v>
+      <c r="C21" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -1579,8 +1587,8 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="21" t="s">
-        <v>43</v>
+      <c r="C22" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -1593,22 +1601,22 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="35"/>
+      <c r="C23" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="21" t="s">
-        <v>44</v>
+      <c r="C24" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -1621,8 +1629,8 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="21" t="s">
-        <v>47</v>
+      <c r="C25" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -1635,16 +1643,16 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
+      <c r="C26" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="29"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
@@ -1675,22 +1683,22 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="29"/>
+      <c r="C29" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="21" t="s">
-        <v>49</v>
+      <c r="C30" s="30" t="s">
+        <v>48</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -1703,8 +1711,8 @@
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="21" t="s">
-        <v>64</v>
+      <c r="C31" s="30" t="s">
+        <v>63</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -1717,22 +1725,22 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="14"/>
-      <c r="C32" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="35"/>
+      <c r="C32" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="14"/>
-      <c r="C33" s="21" t="s">
-        <v>51</v>
+      <c r="C33" s="30" t="s">
+        <v>50</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -1745,8 +1753,8 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="14"/>
-      <c r="C34" s="21" t="s">
-        <v>52</v>
+      <c r="C34" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
@@ -1759,16 +1767,16 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="26"/>
+      <c r="C35" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="29"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
@@ -1786,7 +1794,7 @@
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1799,22 +1807,22 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="14"/>
-      <c r="C38" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="29"/>
+      <c r="C38" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="33"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="14"/>
-      <c r="C39" s="21" t="s">
-        <v>56</v>
+      <c r="C39" s="30" t="s">
+        <v>55</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -1827,7 +1835,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="14"/>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="30" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="22"/>
@@ -1841,22 +1849,22 @@
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="14"/>
-      <c r="C41" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="35"/>
+      <c r="C41" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="26"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="14"/>
-      <c r="C42" s="21" t="s">
-        <v>60</v>
+      <c r="C42" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
@@ -1869,8 +1877,8 @@
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="14"/>
-      <c r="C43" s="21" t="s">
-        <v>28</v>
+      <c r="C43" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -1883,16 +1891,16 @@
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="14"/>
-      <c r="C44" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="26"/>
+      <c r="C44" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
@@ -1910,7 +1918,7 @@
       <c r="A46" s="8"/>
       <c r="B46" s="14"/>
       <c r="C46" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -1923,22 +1931,22 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="11"/>
-      <c r="C47" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="29"/>
+      <c r="C47" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="33"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
-      <c r="C48" s="21" t="s">
-        <v>63</v>
+      <c r="C48" s="30" t="s">
+        <v>62</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -1951,8 +1959,8 @@
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="21" t="s">
-        <v>65</v>
+      <c r="C49" s="30" t="s">
+        <v>64</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -1965,22 +1973,22 @@
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="35"/>
+      <c r="C50" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="26"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="21" t="s">
-        <v>67</v>
+      <c r="C51" s="30" t="s">
+        <v>66</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -1993,8 +2001,8 @@
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="21" t="s">
-        <v>28</v>
+      <c r="C52" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -2007,16 +2015,16 @@
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
-      <c r="C53" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="26"/>
+      <c r="C53" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="29"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
@@ -2034,7 +2042,7 @@
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
@@ -2047,22 +2055,22 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
-      <c r="C56" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="29"/>
+      <c r="C56" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="33"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
-      <c r="C57" s="49" t="s">
-        <v>69</v>
+      <c r="C57" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="22"/>
@@ -2075,8 +2083,8 @@
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
-      <c r="C58" s="49" t="s">
-        <v>68</v>
+      <c r="C58" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
@@ -2087,20 +2095,20 @@
       <c r="J58" s="23"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C59" s="50" t="s">
+      <c r="C59" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="26"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C60" s="21" t="s">
         <v>71</v>
-      </c>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="35"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C60" s="49" t="s">
-        <v>72</v>
       </c>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
@@ -2111,8 +2119,8 @@
       <c r="J60" s="23"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C61" s="49" t="s">
-        <v>73</v>
+      <c r="C61" s="21" t="s">
+        <v>72</v>
       </c>
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
@@ -2123,20 +2131,20 @@
       <c r="J61" s="23"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C62" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="25"/>
-      <c r="J62" s="26"/>
+      <c r="C62" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="29"/>
     </row>
     <row r="64" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="C64" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
@@ -2147,20 +2155,20 @@
       <c r="J64" s="8"/>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C65" s="48" t="s">
+      <c r="C65" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="33"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C66" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="29"/>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C66" s="49" t="s">
-        <v>79</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
@@ -2171,8 +2179,8 @@
       <c r="J66" s="23"/>
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C67" s="49" t="s">
-        <v>80</v>
+      <c r="C67" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
@@ -2183,20 +2191,20 @@
       <c r="J67" s="23"/>
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C68" s="50" t="s">
+      <c r="C68" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="25"/>
+      <c r="H68" s="25"/>
+      <c r="I68" s="25"/>
+      <c r="J68" s="26"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C69" s="21" t="s">
         <v>81</v>
-      </c>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="34"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="34"/>
-      <c r="J68" s="35"/>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C69" s="49" t="s">
-        <v>82</v>
       </c>
       <c r="D69" s="22"/>
       <c r="E69" s="22"/>
@@ -2207,8 +2215,8 @@
       <c r="J69" s="23"/>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C70" s="21" t="s">
-        <v>28</v>
+      <c r="C70" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D70" s="22"/>
       <c r="E70" s="22"/>
@@ -2219,20 +2227,20 @@
       <c r="J70" s="23"/>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C71" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
-      <c r="I71" s="25"/>
-      <c r="J71" s="26"/>
+      <c r="C71" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="29"/>
     </row>
     <row r="73" spans="3:10" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="C73" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
@@ -2243,20 +2251,20 @@
       <c r="J73" s="8"/>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C74" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="29"/>
+      <c r="C74" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="33"/>
     </row>
     <row r="75" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C75" s="49" t="s">
-        <v>84</v>
+      <c r="C75" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="D75" s="22"/>
       <c r="E75" s="22"/>
@@ -2267,8 +2275,8 @@
       <c r="J75" s="23"/>
     </row>
     <row r="76" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C76" s="49" t="s">
-        <v>83</v>
+      <c r="C76" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="D76" s="22"/>
       <c r="E76" s="22"/>
@@ -2279,20 +2287,20 @@
       <c r="J76" s="23"/>
     </row>
     <row r="77" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C77" s="50" t="s">
+      <c r="C77" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="25"/>
+      <c r="I77" s="25"/>
+      <c r="J77" s="26"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C78" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="34"/>
-      <c r="H77" s="34"/>
-      <c r="I77" s="34"/>
-      <c r="J77" s="35"/>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C78" s="49" t="s">
-        <v>87</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="22"/>
@@ -2303,8 +2311,8 @@
       <c r="J78" s="23"/>
     </row>
     <row r="79" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C79" s="21" t="s">
-        <v>28</v>
+      <c r="C79" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22"/>
@@ -2315,20 +2323,20 @@
       <c r="J79" s="23"/>
     </row>
     <row r="80" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C80" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
-      <c r="I80" s="25"/>
-      <c r="J80" s="26"/>
+      <c r="C80" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="29"/>
     </row>
     <row r="82" spans="3:10" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="C82" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
@@ -2339,20 +2347,20 @@
       <c r="J82" s="8"/>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C83" s="48" t="s">
+      <c r="C83" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="32"/>
+      <c r="G83" s="32"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="32"/>
+      <c r="J83" s="33"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C84" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="D83" s="28"/>
-      <c r="E83" s="28"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="28"/>
-      <c r="I83" s="28"/>
-      <c r="J83" s="29"/>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C84" s="49" t="s">
-        <v>89</v>
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="22"/>
@@ -2363,7 +2371,7 @@
       <c r="J84" s="23"/>
     </row>
     <row r="85" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C85" s="21" t="s">
+      <c r="C85" s="30" t="s">
         <v>25</v>
       </c>
       <c r="D85" s="22"/>
@@ -2375,20 +2383,20 @@
       <c r="J85" s="23"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C86" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="D86" s="34"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="34"/>
-      <c r="H86" s="34"/>
-      <c r="I86" s="34"/>
-      <c r="J86" s="35"/>
+      <c r="C86" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="25"/>
+      <c r="H86" s="25"/>
+      <c r="I86" s="25"/>
+      <c r="J86" s="26"/>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C87" s="21" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="D87" s="22"/>
       <c r="E87" s="22"/>
@@ -2399,8 +2407,8 @@
       <c r="J87" s="23"/>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C88" s="21" t="s">
-        <v>28</v>
+      <c r="C88" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D88" s="22"/>
       <c r="E88" s="22"/>
@@ -2411,20 +2419,20 @@
       <c r="J88" s="23"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C89" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="25"/>
-      <c r="H89" s="25"/>
-      <c r="I89" s="25"/>
-      <c r="J89" s="26"/>
+      <c r="C89" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="29"/>
     </row>
     <row r="91" spans="3:10" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="C91" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
@@ -2435,19 +2443,19 @@
       <c r="J91" s="8"/>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C92" s="48" t="s">
+      <c r="C92" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D92" s="28"/>
-      <c r="E92" s="28"/>
-      <c r="F92" s="28"/>
-      <c r="G92" s="28"/>
-      <c r="H92" s="28"/>
-      <c r="I92" s="28"/>
-      <c r="J92" s="29"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="32"/>
+      <c r="F92" s="32"/>
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="32"/>
+      <c r="J92" s="33"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C93" s="49" t="s">
+      <c r="C93" s="21" t="s">
         <v>24</v>
       </c>
       <c r="D93" s="22"/>
@@ -2459,8 +2467,8 @@
       <c r="J93" s="23"/>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C94" s="49" t="s">
-        <v>75</v>
+      <c r="C94" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="D94" s="22"/>
       <c r="E94" s="22"/>
@@ -2471,20 +2479,20 @@
       <c r="J94" s="23"/>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C95" s="50" t="s">
+      <c r="C95" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="34"/>
-      <c r="H95" s="34"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="35"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="25"/>
+      <c r="H95" s="25"/>
+      <c r="I95" s="25"/>
+      <c r="J95" s="26"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C96" s="49" t="s">
-        <v>76</v>
+      <c r="C96" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="D96" s="22"/>
       <c r="E96" s="22"/>
@@ -2495,8 +2503,8 @@
       <c r="J96" s="23"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C97" s="49" t="s">
-        <v>77</v>
+      <c r="C97" s="21" t="s">
+        <v>76</v>
       </c>
       <c r="D97" s="22"/>
       <c r="E97" s="22"/>
@@ -2507,74 +2515,27 @@
       <c r="J97" s="23"/>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C98" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="25"/>
-      <c r="H98" s="25"/>
-      <c r="I98" s="25"/>
-      <c r="J98" s="26"/>
+      <c r="C98" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+      <c r="J98" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="C94:J94"/>
-    <mergeCell ref="C95:J95"/>
-    <mergeCell ref="C96:J96"/>
-    <mergeCell ref="C97:J97"/>
-    <mergeCell ref="C98:J98"/>
-    <mergeCell ref="C87:J87"/>
-    <mergeCell ref="C88:J88"/>
-    <mergeCell ref="C89:J89"/>
-    <mergeCell ref="C92:J92"/>
-    <mergeCell ref="C93:J93"/>
-    <mergeCell ref="C80:J80"/>
-    <mergeCell ref="C83:J83"/>
-    <mergeCell ref="C84:J84"/>
-    <mergeCell ref="C85:J85"/>
-    <mergeCell ref="C86:J86"/>
-    <mergeCell ref="C75:J75"/>
-    <mergeCell ref="C76:J76"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="C78:J78"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="C69:J69"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="C71:J71"/>
-    <mergeCell ref="C74:J74"/>
-    <mergeCell ref="C61:J61"/>
-    <mergeCell ref="C62:J62"/>
-    <mergeCell ref="C65:J65"/>
-    <mergeCell ref="C66:J66"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C56:J56"/>
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="C58:J58"/>
-    <mergeCell ref="C59:J59"/>
-    <mergeCell ref="C60:J60"/>
-    <mergeCell ref="C49:J49"/>
-    <mergeCell ref="C50:J50"/>
-    <mergeCell ref="C51:J51"/>
-    <mergeCell ref="C52:J52"/>
-    <mergeCell ref="C53:J53"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C48:J48"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="C38:J38"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C24:J24"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="C16:D16"/>
@@ -2583,14 +2544,61 @@
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="O10:Q10"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="C49:J49"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C51:J51"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C56:J56"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="C58:J58"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="C60:J60"/>
+    <mergeCell ref="C61:J61"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="C69:J69"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="C71:J71"/>
+    <mergeCell ref="C74:J74"/>
+    <mergeCell ref="C75:J75"/>
+    <mergeCell ref="C76:J76"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="C78:J78"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="C80:J80"/>
+    <mergeCell ref="C83:J83"/>
+    <mergeCell ref="C84:J84"/>
+    <mergeCell ref="C85:J85"/>
+    <mergeCell ref="C86:J86"/>
+    <mergeCell ref="C87:J87"/>
+    <mergeCell ref="C88:J88"/>
+    <mergeCell ref="C89:J89"/>
+    <mergeCell ref="C92:J92"/>
+    <mergeCell ref="C93:J93"/>
+    <mergeCell ref="C94:J94"/>
+    <mergeCell ref="C95:J95"/>
+    <mergeCell ref="C96:J96"/>
+    <mergeCell ref="C97:J97"/>
+    <mergeCell ref="C98:J98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>